<commit_message>
Add fivestand to team reports
</commit_message>
<xml_diff>
--- a/src/main/resources/main-template.xlsx
+++ b/src/main/resources/main-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Busche\Desktop\apps\code\trap-scoring\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrbus\Desktop\code\trap-scoring\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A11B3C-5987-432D-9F0E-A79234C3CAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9016ABC0-9ADC-4F7A-B92E-E86000380BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="36240" windowHeight="23520" tabRatio="672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clean Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Clean Data'!$A$1:$S$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Individual-All-Scores'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Individual-Ladies'!$A$13:$T$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Individual-Ladies'!$B$13:$X$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Individual-Men'!$A$13:$T$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Team-Individual-Scores'!$A$1:$E$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Individual-Ladies'!$A$1:$T$63</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
   <si>
     <t>EventId</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>State League Standings: Individual Ladies</t>
+  </si>
+  <si>
+    <t>Five Stand</t>
   </si>
 </sst>
 </file>
@@ -568,8 +571,8 @@
       <xdr:rowOff>178590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>233305</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>935774</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>26190</xdr:rowOff>
     </xdr:to>
@@ -643,7 +646,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>547639</xdr:colOff>
+      <xdr:colOff>547640</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>7141</xdr:rowOff>
     </xdr:to>
@@ -1017,8 +1020,8 @@
       <xdr:rowOff>178590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>233305</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>935774</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>26190</xdr:rowOff>
     </xdr:to>
@@ -1092,7 +1095,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>547639</xdr:colOff>
+      <xdr:colOff>547640</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>7141</xdr:rowOff>
     </xdr:to>
@@ -2680,7 +2683,7 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B9:N12"/>
+  <dimension ref="B9:Q12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -2701,9 +2704,11 @@
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" customWidth="1"/>
+    <col min="17" max="17" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:14" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:17" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
         <v>28</v>
       </c>
@@ -2720,12 +2725,12 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:14" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:17" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -2740,6 +2745,9 @@
       </c>
       <c r="N12" s="6" t="s">
         <v>22</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2766,7 +2774,7 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B9:N12"/>
+  <dimension ref="B9:Q12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -2787,9 +2795,11 @@
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" customWidth="1"/>
+    <col min="17" max="17" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:14" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:17" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
@@ -2806,12 +2816,12 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:14" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:17" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -2826,6 +2836,9 @@
       </c>
       <c r="N12" s="6" t="s">
         <v>22</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2926,7 +2939,7 @@
   <sheetPr codeName="Sheet4">
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:T13"/>
+  <dimension ref="B1:X13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -2952,65 +2965,77 @@
     <col min="18" max="18" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.7109375" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C1"/>
       <c r="G1"/>
       <c r="K1"/>
       <c r="O1"/>
       <c r="S1"/>
-    </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W1"/>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C2"/>
       <c r="G2"/>
       <c r="K2"/>
       <c r="O2"/>
       <c r="S2"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W2"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C3"/>
       <c r="G3"/>
       <c r="K3"/>
       <c r="O3"/>
       <c r="S3"/>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C4"/>
       <c r="G4"/>
       <c r="K4"/>
       <c r="O4"/>
       <c r="S4"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W4"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C5"/>
       <c r="G5"/>
       <c r="K5"/>
       <c r="O5"/>
       <c r="S5"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W5"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C6"/>
       <c r="G6"/>
       <c r="K6"/>
       <c r="O6"/>
       <c r="S6"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W6"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C7"/>
       <c r="G7"/>
       <c r="K7"/>
       <c r="O7"/>
       <c r="S7"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W7"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C8"/>
       <c r="G8"/>
       <c r="K8"/>
       <c r="O8"/>
       <c r="S8"/>
-    </row>
-    <row r="9" spans="2:20" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="W8"/>
+    </row>
+    <row r="9" spans="2:24" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
         <v>31</v>
       </c>
@@ -3026,8 +3051,9 @@
       <c r="L9" s="9"/>
       <c r="O9"/>
       <c r="S9"/>
-    </row>
-    <row r="10" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="W9"/>
+    </row>
+    <row r="10" spans="2:24" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
@@ -3036,15 +3062,17 @@
       <c r="K10"/>
       <c r="O10"/>
       <c r="S10"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W10"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C11"/>
       <c r="G11"/>
       <c r="K11"/>
       <c r="O11"/>
       <c r="S11"/>
-    </row>
-    <row r="12" spans="2:20" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="W11"/>
+    </row>
+    <row r="12" spans="2:24" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -3060,8 +3088,11 @@
       <c r="R12" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="2:20" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V12" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
@@ -3105,6 +3136,15 @@
         <v>25</v>
       </c>
       <c r="T13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="W13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="X13" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3133,7 +3173,7 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:T13"/>
+  <dimension ref="B1:X13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -3159,65 +3199,77 @@
     <col min="18" max="18" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.7109375" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C1"/>
       <c r="G1"/>
       <c r="K1"/>
       <c r="O1"/>
       <c r="S1"/>
-    </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W1"/>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C2"/>
       <c r="G2"/>
       <c r="K2"/>
       <c r="O2"/>
       <c r="S2"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W2"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C3"/>
       <c r="G3"/>
       <c r="K3"/>
       <c r="O3"/>
       <c r="S3"/>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C4"/>
       <c r="G4"/>
       <c r="K4"/>
       <c r="O4"/>
       <c r="S4"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W4"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C5"/>
       <c r="G5"/>
       <c r="K5"/>
       <c r="O5"/>
       <c r="S5"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W5"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C6"/>
       <c r="G6"/>
       <c r="K6"/>
       <c r="O6"/>
       <c r="S6"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W6"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C7"/>
       <c r="G7"/>
       <c r="K7"/>
       <c r="O7"/>
       <c r="S7"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W7"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C8"/>
       <c r="G8"/>
       <c r="K8"/>
       <c r="O8"/>
       <c r="S8"/>
-    </row>
-    <row r="9" spans="2:20" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="W8"/>
+    </row>
+    <row r="9" spans="2:24" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
         <v>32</v>
       </c>
@@ -3233,8 +3285,9 @@
       <c r="L9" s="9"/>
       <c r="O9"/>
       <c r="S9"/>
-    </row>
-    <row r="10" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="W9"/>
+    </row>
+    <row r="10" spans="2:24" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
@@ -3243,15 +3296,17 @@
       <c r="K10"/>
       <c r="O10"/>
       <c r="S10"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="W10"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C11"/>
       <c r="G11"/>
       <c r="K11"/>
       <c r="O11"/>
       <c r="S11"/>
-    </row>
-    <row r="12" spans="2:20" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="W11"/>
+    </row>
+    <row r="12" spans="2:24" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -3267,8 +3322,11 @@
       <c r="R12" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="2:20" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V12" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
@@ -3314,9 +3372,18 @@
       <c r="T13" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="V13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="W13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A13:T13" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="B13:X13" xr:uid="{E3F3AF09-0935-4B97-AF12-CE1C1B98D7BA}"/>
   <mergeCells count="1">
     <mergeCell ref="B9:L9"/>
   </mergeCells>

</xml_diff>